<commit_message>
Naming convention template file updated
</commit_message>
<xml_diff>
--- a/Naming Convention Template.xlsx
+++ b/Naming Convention Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ethoseng-my.sharepoint.com/personal/rubenslage_ethoseng_ie/Documents/Documents/GitHub/check_file_naming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{3C5A177B-14BD-4D2C-BA6E-808EEE180FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C7175B8-648B-44B5-B27A-54C009AF620B}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{3C5A177B-14BD-4D2C-BA6E-808EEE180FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85CB4065-DAE7-4E82-8CEC-257793DCA2D4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D7ED3C0-DDB4-4BAF-B51C-01B2E7CF43A0}"/>
   </bookViews>
@@ -656,7 +656,7 @@
     <t>CMDI</t>
   </si>
   <si>
-    <t>_</t>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1083,7 @@
   <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>